<commit_message>
Adding More Tests to Hotel Details Page
</commit_message>
<xml_diff>
--- a/TestPlans/Hotel Details Adding Review.xlsx
+++ b/TestPlans/Hotel Details Adding Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PersonalProjects\PHPTravelsNunitFramework\QATesting\TestPlans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D10422B-6806-4D03-A3EE-4D34C532A9A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE5C279-27BE-4B54-8E4D-7CEDAC71E771}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{0EDD3556-9FCE-4929-97F1-67BB33321B97}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Version:</t>
   </si>
@@ -296,6 +296,9 @@
                     "The Email field is required"
                     "The Name field is required"</t>
     </r>
+  </si>
+  <si>
+    <t>pass</t>
   </si>
 </sst>
 </file>
@@ -375,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -390,19 +393,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,13 +765,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{940D422A-8A67-4F8A-8611-6B548BE127B3}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:H26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="54.21875" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5546875" customWidth="1"/>
     <col min="10" max="10" width="26.88671875" customWidth="1"/>
   </cols>
@@ -817,14 +822,14 @@
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
       <c r="I4" s="8" t="s">
         <v>3</v>
       </c>
@@ -858,27 +863,36 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="15">
+        <v>43364</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="15">
+        <v>43364</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -894,11 +908,23 @@
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14" s="15">
+        <v>43364</v>
+      </c>
+      <c r="I14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="B15" s="15">
+        <v>43364</v>
+      </c>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -909,14 +935,14 @@
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -927,14 +953,14 @@
       <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -945,27 +971,27 @@
       <c r="A24" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
     </row>
     <row r="26" spans="1:8" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>